<commit_message>
adds hospital_qunatities serialized data
</commit_message>
<xml_diff>
--- a/execute/import/workbooks/National_Transplant_Hospitals.xlsx
+++ b/execute/import/workbooks/National_Transplant_Hospitals.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1033" uniqueCount="706">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1033" uniqueCount="705">
   <si>
     <t>State</t>
   </si>
@@ -2142,9 +2142,6 @@
   </si>
   <si>
     <t>Tennessee</t>
-  </si>
-  <si>
-    <t>US</t>
   </si>
 </sst>
 </file>
@@ -2690,8 +2687,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N254"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="H42" sqref="H42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3695,8 +3692,8 @@
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46" s="13" t="s">
-        <v>705</v>
+      <c r="A46" s="14" t="s">
+        <v>108</v>
       </c>
       <c r="B46" s="14" t="s">
         <v>109</v>
@@ -3715,8 +3712,8 @@
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A47" s="13" t="s">
-        <v>705</v>
+      <c r="A47" s="14" t="s">
+        <v>108</v>
       </c>
       <c r="B47" s="14" t="s">
         <v>110</v>
@@ -3735,8 +3732,8 @@
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A48" s="13" t="s">
-        <v>705</v>
+      <c r="A48" s="14" t="s">
+        <v>108</v>
       </c>
       <c r="B48" s="14" t="s">
         <v>111</v>
@@ -3755,8 +3752,8 @@
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A49" s="13" t="s">
-        <v>705</v>
+      <c r="A49" s="14" t="s">
+        <v>108</v>
       </c>
       <c r="B49" s="14" t="s">
         <v>112</v>

</xml_diff>